<commit_message>
avance 24 de mayo
</commit_message>
<xml_diff>
--- a/documentos/diccionario.xlsx
+++ b/documentos/diccionario.xlsx
@@ -1100,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A192" sqref="A192:E192"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>